<commit_message>
deploying after variable change
</commit_message>
<xml_diff>
--- a/temp/timesheet_detailed.xlsx
+++ b/temp/timesheet_detailed.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>Username</t>
   </si>
@@ -34,19 +34,10 @@
     <t>29 Aug 24</t>
   </si>
   <si>
-    <t>05:25</t>
-  </si>
-  <si>
-    <t>13:18</t>
-  </si>
-  <si>
-    <t>01 Sept 24</t>
-  </si>
-  <si>
-    <t>20:32</t>
-  </si>
-  <si>
-    <t>03:35</t>
+    <t>13:48</t>
+  </si>
+  <si>
+    <t>17:48</t>
   </si>
   <si>
     <t>Total for yeasir afgan</t>
@@ -55,7 +46,7 @@
     <t/>
   </si>
   <si>
-    <t>14.56</t>
+    <t>4.00</t>
   </si>
   <si>
     <t>Grand Total</t>
@@ -435,11 +426,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="3" width="12" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
   </cols>
@@ -475,24 +467,24 @@
         <v>8</v>
       </c>
       <c r="E2">
-        <v>7.53</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
       <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
         <v>11</v>
-      </c>
-      <c r="E3">
-        <v>7.03</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -500,33 +492,16 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>